<commit_message>
Minor changes and Interventions runned in large scale mode
</commit_message>
<xml_diff>
--- a/Ecopulpers/Baseline Results/Ecopulpers - baseline.xlsx
+++ b/Ecopulpers/Baseline Results/Ecopulpers - baseline.xlsx
@@ -613,70 +613,70 @@
         <v>29</v>
       </c>
       <c r="C4">
-        <v>0.9999999161809683</v>
+        <v>96.95999200548977</v>
       </c>
       <c r="D4">
-        <v>0.5301520954817533</v>
+        <v>51.40427538286895</v>
       </c>
       <c r="E4">
-        <v>0.5301521399185923</v>
+        <v>0.5301596495589489</v>
       </c>
       <c r="F4">
-        <v>1.886250992316197</v>
+        <v>1.886224273823784</v>
       </c>
       <c r="G4">
-        <v>1.456106646044645</v>
+        <v>141.1196250437642</v>
       </c>
       <c r="H4">
-        <v>0.0002509020414436236</v>
+        <v>0.02433365207616589</v>
       </c>
       <c r="I4">
-        <v>0.003194511628862529</v>
+        <v>0.3097206776392341</v>
       </c>
       <c r="J4">
-        <v>0.04977364698424935</v>
+        <v>4.825945775955915</v>
       </c>
       <c r="K4">
-        <v>0.01479718252085149</v>
+        <v>1.434611532604322</v>
       </c>
       <c r="L4">
-        <v>0.05799348698928952</v>
+        <v>5.622603700961918</v>
       </c>
       <c r="M4">
-        <v>0.002247946278657764</v>
+        <v>0.2179608714068308</v>
       </c>
       <c r="N4">
-        <v>0.002062287945591379</v>
+        <v>0.1999594387507386</v>
       </c>
       <c r="O4">
-        <v>8.982479812402744e-06</v>
+        <v>0.0008709411613381235</v>
       </c>
       <c r="P4">
-        <v>0.2918828048277646</v>
+        <v>28.30095673212782</v>
       </c>
       <c r="Q4">
-        <v>0.05669153109192848</v>
+        <v>5.496810862794518</v>
       </c>
       <c r="R4">
-        <v>0.5284182245377451</v>
+        <v>51.23543111188337</v>
       </c>
       <c r="S4">
-        <v>-14.5588185141678</v>
+        <v>-1410.978289566236</v>
       </c>
       <c r="T4">
-        <v>-0.0004467324688448571</v>
+        <v>-0.04337708201092028</v>
       </c>
       <c r="U4">
-        <v>-0.03193613380881288</v>
+        <v>-3.096335835231002</v>
       </c>
       <c r="V4">
-        <v>-0.2058536650147289</v>
+        <v>-19.95850102743134</v>
       </c>
       <c r="W4">
-        <v>-0.5232433388009667</v>
+        <v>-50.72922614682466</v>
       </c>
       <c r="X4">
-        <v>0.3804463993292302</v>
+        <v>36.88931578584015</v>
       </c>
     </row>
   </sheetData>

</xml_diff>